<commit_message>
feat: various adjustments to the datasets
</commit_message>
<xml_diff>
--- a/datasets/combined_dataset.xlsx
+++ b/datasets/combined_dataset.xlsx
@@ -1253,27 +1253,27 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Default</t>
+          <t>Tale</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>28</v>
+        <v>744</v>
       </c>
       <c r="D33" t="n">
-        <v>316</v>
+        <v>4631</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5316455696202531</v>
+        <v>0.9529259339235586</v>
       </c>
       <c r="F33" t="n">
-        <v>6</v>
+        <v>5.931451612903226</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>45485.9921412037</v>
+        <v>45801.52984953704</v>
       </c>
     </row>
     <row r="34">
@@ -1461,19 +1461,19 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>157268</v>
+        <v>165216</v>
       </c>
       <c r="D41" t="n">
-        <v>1008504</v>
+        <v>1058861</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9757135321228276</v>
+        <v>0.976415223527923</v>
       </c>
       <c r="F41" t="n">
-        <v>6.256905409873592</v>
+        <v>6.257795855122991</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>45793.91333333333</v>
+        <v>45801.56623842593</v>
       </c>
     </row>
     <row r="42">
@@ -1882,23 +1882,23 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Subcategory</t>
+          <t>Tale</t>
         </is>
       </c>
       <c r="C58" t="n">
         <v>2244</v>
       </c>
       <c r="D58" t="n">
-        <v>13959</v>
+        <v>13886</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9835231750125368</v>
+        <v>0.988693648278842</v>
       </c>
       <c r="F58" t="n">
         <v>6.118092691622104</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>45522.73387731481</v>
+        <v>45801.53</v>
       </c>
     </row>
     <row r="59">
@@ -2112,7 +2112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G236"/>
+  <dimension ref="A1:G240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2173,10 +2173,10 @@
         <v>2148</v>
       </c>
       <c r="E2" t="n">
-        <v>6.144</v>
+        <v>6.1437125748503</v>
       </c>
       <c r="F2" t="n">
-        <v>0.955</v>
+        <v>0.9553072625698324</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>45289.79652777778</v>
@@ -2198,10 +2198,10 @@
         <v>3902</v>
       </c>
       <c r="E3" t="n">
-        <v>6.606</v>
+        <v>6.606007067137809</v>
       </c>
       <c r="F3" t="n">
-        <v>0.958</v>
+        <v>0.9582265504869296</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>45289.66180555556</v>
@@ -2223,10 +2223,10 @@
         <v>2113</v>
       </c>
       <c r="E4" t="n">
-        <v>6.424</v>
+        <v>6.423780487804878</v>
       </c>
       <c r="F4" t="n">
-        <v>0.997</v>
+        <v>0.9971604353999054</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>45289.74305555555</v>
@@ -2248,10 +2248,10 @@
         <v>6737</v>
       </c>
       <c r="E5" t="n">
-        <v>6.405</v>
+        <v>6.404761904761905</v>
       </c>
       <c r="F5" t="n">
-        <v>0.998</v>
+        <v>0.9982187917470684</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>45745.725</v>
@@ -2273,10 +2273,10 @@
         <v>2566</v>
       </c>
       <c r="E6" t="n">
-        <v>6.259</v>
+        <v>6.25916870415648</v>
       </c>
       <c r="F6" t="n">
-        <v>0.998</v>
+        <v>0.9976617303195636</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>45287.73888888889</v>
@@ -2301,7 +2301,7 @@
         <v>5.875</v>
       </c>
       <c r="F7" t="n">
-        <v>0.96</v>
+        <v>0.9598960267359822</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>45285.66736111111</v>
@@ -2323,10 +2323,10 @@
         <v>1940</v>
       </c>
       <c r="E8" t="n">
-        <v>6.025</v>
+        <v>6.024922118380062</v>
       </c>
       <c r="F8" t="n">
-        <v>0.997</v>
+        <v>0.9969072164948454</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>45285.63819444444</v>
@@ -2348,10 +2348,10 @@
         <v>2645</v>
       </c>
       <c r="E9" t="n">
-        <v>6.053</v>
+        <v>6.052752293577981</v>
       </c>
       <c r="F9" t="n">
-        <v>0.998</v>
+        <v>0.9977315689981096</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>45285.64236111111</v>
@@ -2373,10 +2373,10 @@
         <v>7465</v>
       </c>
       <c r="E10" t="n">
-        <v>6.284</v>
+        <v>6.284388185654008</v>
       </c>
       <c r="F10" t="n">
-        <v>0.998</v>
+        <v>0.9975887474882786</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>45283.96805555555</v>
@@ -2398,10 +2398,10 @@
         <v>1711</v>
       </c>
       <c r="E11" t="n">
-        <v>5.78</v>
+        <v>5.779661016949152</v>
       </c>
       <c r="F11" t="n">
-        <v>0.996</v>
+        <v>0.9964932787843368</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>45283.76527777778</v>
@@ -2423,10 +2423,10 @@
         <v>1745</v>
       </c>
       <c r="E12" t="n">
-        <v>6.189</v>
+        <v>6.188612099644129</v>
       </c>
       <c r="F12" t="n">
-        <v>0.997</v>
+        <v>0.9965616045845272</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>45283.79236111111</v>
@@ -2448,10 +2448,10 @@
         <v>2464</v>
       </c>
       <c r="E13" t="n">
-        <v>5.857</v>
+        <v>5.856801909307876</v>
       </c>
       <c r="F13" t="n">
-        <v>0.996</v>
+        <v>0.9959415584415584</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>45283.25208333333</v>
@@ -2473,10 +2473,10 @@
         <v>1645</v>
       </c>
       <c r="E14" t="n">
-        <v>6.185</v>
+        <v>6.184905660377359</v>
       </c>
       <c r="F14" t="n">
-        <v>0.996</v>
+        <v>0.9963525835866262</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>45283.68958333333</v>
@@ -2498,10 +2498,10 @@
         <v>1822</v>
       </c>
       <c r="E15" t="n">
-        <v>6.262</v>
+        <v>6.262068965517241</v>
       </c>
       <c r="F15" t="n">
-        <v>0.997</v>
+        <v>0.9967069154774972</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>45282.78125</v>
@@ -2523,10 +2523,10 @@
         <v>1103</v>
       </c>
       <c r="E16" t="n">
-        <v>6.349</v>
+        <v>6.349397590361446</v>
       </c>
       <c r="F16" t="n">
-        <v>0.956</v>
+        <v>0.9555757026291932</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>45280.77847222222</v>
@@ -2548,10 +2548,10 @@
         <v>13549</v>
       </c>
       <c r="E17" t="n">
-        <v>6.483</v>
+        <v>6.482507288629738</v>
       </c>
       <c r="F17" t="n">
-        <v>0.985</v>
+        <v>0.9846483135286735</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>45278.73888888889</v>
@@ -2573,10 +2573,10 @@
         <v>3197</v>
       </c>
       <c r="E18" t="n">
-        <v>6.539</v>
+        <v>6.538934426229508</v>
       </c>
       <c r="F18" t="n">
-        <v>0.998</v>
+        <v>0.9981232405380044</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>45275.32430555556</v>
@@ -2598,10 +2598,10 @@
         <v>3766</v>
       </c>
       <c r="E19" t="n">
-        <v>6.14</v>
+        <v>6.139767054908486</v>
       </c>
       <c r="F19" t="n">
-        <v>0.98</v>
+        <v>0.9798194370685076</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>45273.85555555556</v>
@@ -2623,10 +2623,10 @@
         <v>4068</v>
       </c>
       <c r="E20" t="n">
-        <v>6.063</v>
+        <v>6.062686567164179</v>
       </c>
       <c r="F20" t="n">
-        <v>0.999</v>
+        <v>0.9985250737463128</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>45270.72013888889</v>
@@ -2648,10 +2648,10 @@
         <v>8588</v>
       </c>
       <c r="E21" t="n">
-        <v>5.959</v>
+        <v>5.959269662921348</v>
       </c>
       <c r="F21" t="n">
-        <v>0.988</v>
+        <v>0.9881229622729388</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>45265.80833333333</v>
@@ -2673,10 +2673,10 @@
         <v>13145</v>
       </c>
       <c r="E22" t="n">
-        <v>5.876</v>
+        <v>5.875736961451247</v>
       </c>
       <c r="F22" t="n">
-        <v>0.986</v>
+        <v>0.9856219094712818</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>45265.46875</v>
@@ -2698,10 +2698,10 @@
         <v>3247</v>
       </c>
       <c r="E23" t="n">
-        <v>6.006</v>
+        <v>6.00556586270872</v>
       </c>
       <c r="F23" t="n">
-        <v>0.997</v>
+        <v>0.9969202340622112</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>45263.39722222222</v>
@@ -2723,10 +2723,10 @@
         <v>4893</v>
       </c>
       <c r="E24" t="n">
-        <v>6.094</v>
+        <v>6.093516209476309</v>
       </c>
       <c r="F24" t="n">
-        <v>0.999</v>
+        <v>0.9987737584304108</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>45262.85763888889</v>
@@ -2748,10 +2748,10 @@
         <v>4785</v>
       </c>
       <c r="E25" t="n">
-        <v>6.306</v>
+        <v>6.305960264900662</v>
       </c>
       <c r="F25" t="n">
-        <v>0.995</v>
+        <v>0.9949843260188088</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>45259.32708333333</v>
@@ -2773,10 +2773,10 @@
         <v>4047</v>
       </c>
       <c r="E26" t="n">
-        <v>6.132</v>
+        <v>6.132018209408194</v>
       </c>
       <c r="F26" t="n">
-        <v>0.999</v>
+        <v>0.9985174203113416</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>45257.48958333334</v>
@@ -2798,10 +2798,10 @@
         <v>2002</v>
       </c>
       <c r="E27" t="n">
-        <v>6.16</v>
+        <v>6.160493827160494</v>
       </c>
       <c r="F27" t="n">
-        <v>0.997</v>
+        <v>0.997002997002997</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>45254.77291666667</v>
@@ -2823,10 +2823,10 @@
         <v>6750</v>
       </c>
       <c r="E28" t="n">
-        <v>6.16</v>
+        <v>6.160482374768089</v>
       </c>
       <c r="F28" t="n">
-        <v>0.984</v>
+        <v>0.983851851851852</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>45254.74236111111</v>
@@ -2848,10 +2848,10 @@
         <v>839</v>
       </c>
       <c r="E29" t="n">
-        <v>6.051</v>
+        <v>6.051094890510949</v>
       </c>
       <c r="F29" t="n">
-        <v>0.988</v>
+        <v>0.9880810488676997</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>45249.66388888889</v>
@@ -2873,10 +2873,10 @@
         <v>7674</v>
       </c>
       <c r="E30" t="n">
-        <v>5.912</v>
+        <v>5.912104857363146</v>
       </c>
       <c r="F30" t="n">
-        <v>0.999</v>
+        <v>0.9992181391712276</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>45242.85833333333</v>
@@ -2898,10 +2898,10 @@
         <v>3729</v>
       </c>
       <c r="E31" t="n">
-        <v>6.164</v>
+        <v>6.163907284768212</v>
       </c>
       <c r="F31" t="n">
-        <v>0.998</v>
+        <v>0.998390989541432</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>45239.75625</v>
@@ -2923,10 +2923,10 @@
         <v>1330</v>
       </c>
       <c r="E32" t="n">
-        <v>6.427</v>
+        <v>6.427184466019417</v>
       </c>
       <c r="F32" t="n">
-        <v>0.995</v>
+        <v>0.9954887218045112</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>45279.35069444445</v>
@@ -2948,10 +2948,10 @@
         <v>2723</v>
       </c>
       <c r="E33" t="n">
-        <v>6.144</v>
+        <v>6.144208037825059</v>
       </c>
       <c r="F33" t="n">
-        <v>0.954</v>
+        <v>0.9544619904517077</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>45293.42638888889</v>
@@ -2973,10 +2973,10 @@
         <v>1968</v>
       </c>
       <c r="E34" t="n">
-        <v>5.892</v>
+        <v>5.891891891891892</v>
       </c>
       <c r="F34" t="n">
-        <v>0.997</v>
+        <v>0.9969512195121952</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>45293.73194444444</v>
@@ -2998,10 +2998,10 @@
         <v>3715</v>
       </c>
       <c r="E35" t="n">
-        <v>6.011</v>
+        <v>6.011345218800648</v>
       </c>
       <c r="F35" t="n">
-        <v>0.998</v>
+        <v>0.998384925975774</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>45294.72638888889</v>
@@ -3023,10 +3023,10 @@
         <v>4528</v>
       </c>
       <c r="E36" t="n">
-        <v>6.158</v>
+        <v>6.15818431911967</v>
       </c>
       <c r="F36" t="n">
-        <v>0.989</v>
+        <v>0.9887367491166078</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>45295.60625</v>
@@ -3048,10 +3048,10 @@
         <v>5348</v>
       </c>
       <c r="E37" t="n">
-        <v>6.314</v>
+        <v>6.314420803782506</v>
       </c>
       <c r="F37" t="n">
-        <v>0.999</v>
+        <v>0.9988780852655198</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>45296.62361111111</v>
@@ -3076,7 +3076,7 @@
         <v>6.125</v>
       </c>
       <c r="F38" t="n">
-        <v>0.997</v>
+        <v>0.9965136548518304</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>45296.66319444445</v>
@@ -3098,10 +3098,10 @@
         <v>12856</v>
       </c>
       <c r="E39" t="n">
-        <v>6.14</v>
+        <v>6.139512661251792</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>0.9995332918481644</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>45297.62708333333</v>
@@ -3123,10 +3123,10 @@
         <v>1273</v>
       </c>
       <c r="E40" t="n">
-        <v>6.211</v>
+        <v>6.21078431372549</v>
       </c>
       <c r="F40" t="n">
-        <v>0.995</v>
+        <v>0.9952867242733699</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>45297.71041666667</v>
@@ -3148,10 +3148,10 @@
         <v>2149</v>
       </c>
       <c r="E41" t="n">
-        <v>6.088</v>
+        <v>6.088068181818182</v>
       </c>
       <c r="F41" t="n">
-        <v>0.997</v>
+        <v>0.9972080037226616</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>45297.71666666667</v>
@@ -3173,10 +3173,10 @@
         <v>1651</v>
       </c>
       <c r="E42" t="n">
-        <v>6.279</v>
+        <v>6.278625954198473</v>
       </c>
       <c r="F42" t="n">
-        <v>0.996</v>
+        <v>0.996365838885524</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>45297.725</v>
@@ -3198,10 +3198,10 @@
         <v>2027</v>
       </c>
       <c r="E43" t="n">
-        <v>6.199</v>
+        <v>6.199386503067485</v>
       </c>
       <c r="F43" t="n">
-        <v>0.997</v>
+        <v>0.9970399605328072</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>45297.73333333333</v>
@@ -3223,10 +3223,10 @@
         <v>1374</v>
       </c>
       <c r="E44" t="n">
-        <v>5.922</v>
+        <v>5.922077922077922</v>
       </c>
       <c r="F44" t="n">
-        <v>0.996</v>
+        <v>0.9956331877729258</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>45297.79305555556</v>
@@ -3248,10 +3248,10 @@
         <v>1726</v>
       </c>
       <c r="E45" t="n">
-        <v>5.85</v>
+        <v>5.850340136054422</v>
       </c>
       <c r="F45" t="n">
-        <v>0.997</v>
+        <v>0.996523754345307</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>45298.6</v>
@@ -3273,10 +3273,10 @@
         <v>2073</v>
       </c>
       <c r="E46" t="n">
-        <v>6.419</v>
+        <v>6.419254658385094</v>
       </c>
       <c r="F46" t="n">
-        <v>0.997</v>
+        <v>0.9971056439942112</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>45298.61736111111</v>
@@ -3298,10 +3298,10 @@
         <v>1787</v>
       </c>
       <c r="E47" t="n">
-        <v>6.154</v>
+        <v>6.154135338345864</v>
       </c>
       <c r="F47" t="n">
-        <v>0.916</v>
+        <v>0.9160604364857304</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>45298.63263888889</v>
@@ -3323,10 +3323,10 @@
         <v>2358</v>
       </c>
       <c r="E48" t="n">
-        <v>6.391</v>
+        <v>6.39067055393586</v>
       </c>
       <c r="F48" t="n">
-        <v>0.93</v>
+        <v>0.9296013570822732</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>45298.64375</v>
@@ -3348,10 +3348,10 @@
         <v>1765</v>
       </c>
       <c r="E49" t="n">
-        <v>6.194</v>
+        <v>6.193661971830986</v>
       </c>
       <c r="F49" t="n">
-        <v>0.997</v>
+        <v>0.9966005665722379</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>45298.65138888889</v>
@@ -3373,10 +3373,10 @@
         <v>3308</v>
       </c>
       <c r="E50" t="n">
-        <v>6.092</v>
+        <v>6.092250922509225</v>
       </c>
       <c r="F50" t="n">
-        <v>0.998</v>
+        <v>0.998186215235792</v>
       </c>
       <c r="G50" s="2" t="n">
         <v>44934.70486111111</v>
@@ -3398,10 +3398,10 @@
         <v>1846</v>
       </c>
       <c r="E51" t="n">
-        <v>6.309</v>
+        <v>6.309278350515464</v>
       </c>
       <c r="F51" t="n">
-        <v>0.995</v>
+        <v>0.9945828819068256</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>45299.72361111111</v>
@@ -3423,10 +3423,10 @@
         <v>3166</v>
       </c>
       <c r="E52" t="n">
-        <v>6.077</v>
+        <v>6.077220077220077</v>
       </c>
       <c r="F52" t="n">
-        <v>0.994</v>
+        <v>0.9943145925457992</v>
       </c>
       <c r="G52" s="2" t="n">
         <v>45299.73888888889</v>
@@ -3448,10 +3448,10 @@
         <v>5255</v>
       </c>
       <c r="E53" t="n">
-        <v>5.958</v>
+        <v>5.95800227014756</v>
       </c>
       <c r="F53" t="n">
-        <v>0.999</v>
+        <v>0.9988582302568982</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>45299.75347222222</v>
@@ -3473,10 +3473,10 @@
         <v>1856</v>
       </c>
       <c r="E54" t="n">
-        <v>6.229</v>
+        <v>6.228956228956229</v>
       </c>
       <c r="F54" t="n">
-        <v>0.997</v>
+        <v>0.9967672413793104</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>45299.78194444445</v>
@@ -3498,10 +3498,10 @@
         <v>8432</v>
       </c>
       <c r="E55" t="n">
-        <v>5.993</v>
+        <v>5.992857142857143</v>
       </c>
       <c r="F55" t="n">
-        <v>0.995</v>
+        <v>0.9950189753320684</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>45300.73888888889</v>
@@ -3523,10 +3523,10 @@
         <v>7867</v>
       </c>
       <c r="E56" t="n">
-        <v>5.963</v>
+        <v>5.962794229309036</v>
       </c>
       <c r="F56" t="n">
-        <v>0.998</v>
+        <v>0.9982204143892208</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>45300.78194444445</v>
@@ -3548,10 +3548,10 @@
         <v>1909</v>
       </c>
       <c r="E57" t="n">
-        <v>7.541</v>
+        <v>7.541463414634146</v>
       </c>
       <c r="F57" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.8098480880041907</v>
       </c>
       <c r="G57" s="2" t="n">
         <v>45300.79583333333</v>
@@ -3573,10 +3573,10 @@
         <v>2190</v>
       </c>
       <c r="E58" t="n">
-        <v>6.101</v>
+        <v>6.101226993865031</v>
       </c>
       <c r="F58" t="n">
-        <v>0.908</v>
+        <v>0.9082191780821918</v>
       </c>
       <c r="G58" s="2" t="n">
         <v>45301.80902777778</v>
@@ -3598,10 +3598,10 @@
         <v>4007</v>
       </c>
       <c r="E59" t="n">
-        <v>6.064</v>
+        <v>6.063664596273292</v>
       </c>
       <c r="F59" t="n">
-        <v>0.975</v>
+        <v>0.9745445470426752</v>
       </c>
       <c r="G59" s="2" t="n">
         <v>45302.74236111111</v>
@@ -3623,10 +3623,10 @@
         <v>1716</v>
       </c>
       <c r="E60" t="n">
-        <v>6.151</v>
+        <v>6.151079136690647</v>
       </c>
       <c r="F60" t="n">
-        <v>0.997</v>
+        <v>0.9965034965034965</v>
       </c>
       <c r="G60" s="2" t="n">
         <v>45302.78472222222</v>
@@ -3648,10 +3648,10 @@
         <v>964</v>
       </c>
       <c r="E61" t="n">
-        <v>6.517</v>
+        <v>6.517006802721088</v>
       </c>
       <c r="F61" t="n">
-        <v>0.994</v>
+        <v>0.9937759336099584</v>
       </c>
       <c r="G61" s="2" t="n">
         <v>45304.63888888889</v>
@@ -3673,10 +3673,10 @@
         <v>1154</v>
       </c>
       <c r="E62" t="n">
-        <v>6.523</v>
+        <v>6.522727272727272</v>
       </c>
       <c r="F62" t="n">
-        <v>0.995</v>
+        <v>0.9948006932409011</v>
       </c>
       <c r="G62" s="2" t="n">
         <v>45304.63888888889</v>
@@ -3698,10 +3698,10 @@
         <v>3877</v>
       </c>
       <c r="E63" t="n">
-        <v>6.506</v>
+        <v>6.505882352941176</v>
       </c>
       <c r="F63" t="n">
-        <v>0.998</v>
+        <v>0.9984524116584989</v>
       </c>
       <c r="G63" s="2" t="n">
         <v>45304.66666666666</v>
@@ -3723,10 +3723,10 @@
         <v>2409</v>
       </c>
       <c r="E64" t="n">
-        <v>6.099</v>
+        <v>6.098984771573604</v>
       </c>
       <c r="F64" t="n">
-        <v>0.998</v>
+        <v>0.9975093399750934</v>
       </c>
       <c r="G64" s="2" t="n">
         <v>45304.77222222222</v>
@@ -3748,10 +3748,10 @@
         <v>4885</v>
       </c>
       <c r="E65" t="n">
-        <v>6.13</v>
+        <v>6.130490956072351</v>
       </c>
       <c r="F65" t="n">
-        <v>0.971</v>
+        <v>0.9713408393039918</v>
       </c>
       <c r="G65" s="2" t="n">
         <v>45306.75486111111</v>
@@ -3773,10 +3773,10 @@
         <v>1881</v>
       </c>
       <c r="E66" t="n">
-        <v>6.461</v>
+        <v>6.461267605633803</v>
       </c>
       <c r="F66" t="n">
-        <v>0.976</v>
+        <v>0.975544922913344</v>
       </c>
       <c r="G66" s="2" t="n">
         <v>45306.79930555556</v>
@@ -3798,10 +3798,10 @@
         <v>1603</v>
       </c>
       <c r="E67" t="n">
-        <v>6.433</v>
+        <v>6.433333333333334</v>
       </c>
       <c r="F67" t="n">
-        <v>0.963</v>
+        <v>0.9631940112289458</v>
       </c>
       <c r="G67" s="2" t="n">
         <v>45306.80763888889</v>
@@ -3823,10 +3823,10 @@
         <v>1761</v>
       </c>
       <c r="E68" t="n">
-        <v>6.138</v>
+        <v>6.138297872340425</v>
       </c>
       <c r="F68" t="n">
-        <v>0.983</v>
+        <v>0.9829642248722316</v>
       </c>
       <c r="G68" s="2" t="n">
         <v>45306.81388888889</v>
@@ -3848,10 +3848,10 @@
         <v>1711</v>
       </c>
       <c r="E69" t="n">
-        <v>6.394</v>
+        <v>6.393822393822393</v>
       </c>
       <c r="F69" t="n">
-        <v>0.968</v>
+        <v>0.967855055523086</v>
       </c>
       <c r="G69" s="2" t="n">
         <v>45310.77222222222</v>
@@ -3876,7 +3876,7 @@
         <v>6.9</v>
       </c>
       <c r="F70" t="n">
-        <v>0.929</v>
+        <v>0.9286132241076652</v>
       </c>
       <c r="G70" s="2" t="n">
         <v>45310.77916666667</v>
@@ -3898,10 +3898,10 @@
         <v>988</v>
       </c>
       <c r="E71" t="n">
-        <v>6.093</v>
+        <v>6.093333333333334</v>
       </c>
       <c r="F71" t="n">
-        <v>0.925</v>
+        <v>0.9251012145748988</v>
       </c>
       <c r="G71" s="2" t="n">
         <v>45310.78888888889</v>
@@ -3923,10 +3923,10 @@
         <v>525</v>
       </c>
       <c r="E72" t="n">
-        <v>6.253</v>
+        <v>6.253012048192771</v>
       </c>
       <c r="F72" t="n">
-        <v>0.989</v>
+        <v>0.9885714285714284</v>
       </c>
       <c r="G72" s="2" t="n">
         <v>45310.79166666666</v>
@@ -3948,10 +3948,10 @@
         <v>1066</v>
       </c>
       <c r="E73" t="n">
-        <v>6.235</v>
+        <v>6.235294117647059</v>
       </c>
       <c r="F73" t="n">
-        <v>0.994</v>
+        <v>0.9943714821763602</v>
       </c>
       <c r="G73" s="2" t="n">
         <v>45311.77222222222</v>
@@ -3973,10 +3973,10 @@
         <v>7933</v>
       </c>
       <c r="E74" t="n">
-        <v>6.442</v>
+        <v>6.442182410423452</v>
       </c>
       <c r="F74" t="n">
-        <v>0.997</v>
+        <v>0.9972267742342116</v>
       </c>
       <c r="G74" s="2" t="n">
         <v>45312.79444444444</v>
@@ -3998,10 +3998,10 @@
         <v>2072</v>
       </c>
       <c r="E75" t="n">
-        <v>6.416</v>
+        <v>6.416149068322981</v>
       </c>
       <c r="F75" t="n">
-        <v>0.997</v>
+        <v>0.9971042471042471</v>
       </c>
       <c r="G75" s="2" t="n">
         <v>45312.86597222222</v>
@@ -4023,10 +4023,10 @@
         <v>1197</v>
       </c>
       <c r="E76" t="n">
-        <v>6.58</v>
+        <v>6.580110497237569</v>
       </c>
       <c r="F76" t="n">
-        <v>0.995</v>
+        <v>0.9949874686716792</v>
       </c>
       <c r="G76" s="2" t="n">
         <v>45312.98888888889</v>
@@ -4048,10 +4048,10 @@
         <v>1647</v>
       </c>
       <c r="E77" t="n">
-        <v>6.146</v>
+        <v>6.146067415730337</v>
       </c>
       <c r="F77" t="n">
-        <v>0.996</v>
+        <v>0.9963570127504554</v>
       </c>
       <c r="G77" s="2" t="n">
         <v>45313.60069444445</v>
@@ -4073,10 +4073,10 @@
         <v>2235</v>
       </c>
       <c r="E78" t="n">
-        <v>5.835</v>
+        <v>5.835078534031414</v>
       </c>
       <c r="F78" t="n">
-        <v>0.997</v>
+        <v>0.9973154362416108</v>
       </c>
       <c r="G78" s="2" t="n">
         <v>45316.36736111111</v>
@@ -4098,10 +4098,10 @@
         <v>2075</v>
       </c>
       <c r="E79" t="n">
-        <v>5.878</v>
+        <v>5.877840909090909</v>
       </c>
       <c r="F79" t="n">
-        <v>0.997</v>
+        <v>0.9971084337349396</v>
       </c>
       <c r="G79" s="2" t="n">
         <v>45316.77222222222</v>
@@ -4123,10 +4123,10 @@
         <v>1596</v>
       </c>
       <c r="E80" t="n">
-        <v>6.08</v>
+        <v>6.079646017699115</v>
       </c>
       <c r="F80" t="n">
-        <v>0.861</v>
+        <v>0.8609022556390977</v>
       </c>
       <c r="G80" s="2" t="n">
         <v>45317.57638888889</v>
@@ -4148,10 +4148,10 @@
         <v>1168</v>
       </c>
       <c r="E81" t="n">
-        <v>6.052</v>
+        <v>6.052083333333333</v>
       </c>
       <c r="F81" t="n">
-        <v>0.995</v>
+        <v>0.9948630136986302</v>
       </c>
       <c r="G81" s="2" t="n">
         <v>45317.58402777778</v>
@@ -4173,10 +4173,10 @@
         <v>4230</v>
       </c>
       <c r="E82" t="n">
-        <v>6.64</v>
+        <v>6.639802631578948</v>
       </c>
       <c r="F82" t="n">
-        <v>0.954</v>
+        <v>0.9543735224586288</v>
       </c>
       <c r="G82" s="2" t="n">
         <v>45318.69513888889</v>
@@ -4198,10 +4198,10 @@
         <v>2165</v>
       </c>
       <c r="E83" t="n">
-        <v>6.234</v>
+        <v>6.233644859813084</v>
       </c>
       <c r="F83" t="n">
-        <v>0.924</v>
+        <v>0.9242494226327944</v>
       </c>
       <c r="G83" s="2" t="n">
         <v>45319.87986111111</v>
@@ -4223,10 +4223,10 @@
         <v>1795</v>
       </c>
       <c r="E84" t="n">
-        <v>6.148</v>
+        <v>6.147766323024055</v>
       </c>
       <c r="F84" t="n">
-        <v>0.997</v>
+        <v>0.9966573816155988</v>
       </c>
       <c r="G84" s="2" t="n">
         <v>45320.73472222222</v>
@@ -4248,10 +4248,10 @@
         <v>4076</v>
       </c>
       <c r="E85" t="n">
-        <v>6.157</v>
+        <v>6.157337367624811</v>
       </c>
       <c r="F85" t="n">
-        <v>0.999</v>
+        <v>0.9985279685966634</v>
       </c>
       <c r="G85" s="2" t="n">
         <v>45323.65833333333</v>
@@ -4273,10 +4273,10 @@
         <v>2130</v>
       </c>
       <c r="E86" t="n">
-        <v>5.787</v>
+        <v>5.787465940054496</v>
       </c>
       <c r="F86" t="n">
-        <v>0.997</v>
+        <v>0.9971830985915492</v>
       </c>
       <c r="G86" s="2" t="n">
         <v>45324.72222222222</v>
@@ -4298,10 +4298,10 @@
         <v>1689</v>
       </c>
       <c r="E87" t="n">
-        <v>6.705</v>
+        <v>6.705179282868526</v>
       </c>
       <c r="F87" t="n">
-        <v>0.996</v>
+        <v>0.9964476021314388</v>
       </c>
       <c r="G87" s="2" t="n">
         <v>45327.74166666667</v>
@@ -4323,10 +4323,10 @@
         <v>1248</v>
       </c>
       <c r="E88" t="n">
-        <v>7.324</v>
+        <v>7.323943661971831</v>
       </c>
       <c r="F88" t="n">
-        <v>0.833</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G88" s="2" t="n">
         <v>45328.44097222222</v>
@@ -4348,10 +4348,10 @@
         <v>2059</v>
       </c>
       <c r="E89" t="n">
-        <v>5.866</v>
+        <v>5.865714285714286</v>
       </c>
       <c r="F89" t="n">
-        <v>0.997</v>
+        <v>0.9970859640602234</v>
       </c>
       <c r="G89" s="2" t="n">
         <v>45328.48819444444</v>
@@ -4373,10 +4373,10 @@
         <v>2547</v>
       </c>
       <c r="E90" t="n">
-        <v>5.571</v>
+        <v>5.571428571428571</v>
       </c>
       <c r="F90" t="n">
-        <v>0.98</v>
+        <v>0.9799764428739692</v>
       </c>
       <c r="G90" s="2" t="n">
         <v>45328.50486111111</v>
@@ -4398,10 +4398,10 @@
         <v>1782</v>
       </c>
       <c r="E91" t="n">
-        <v>5.94</v>
+        <v>5.939799331103679</v>
       </c>
       <c r="F91" t="n">
-        <v>0.997</v>
+        <v>0.9966329966329966</v>
       </c>
       <c r="G91" s="2" t="n">
         <v>45328.66180555556</v>
@@ -4423,10 +4423,10 @@
         <v>4596</v>
       </c>
       <c r="E92" t="n">
-        <v>6.538</v>
+        <v>6.538461538461538</v>
       </c>
       <c r="F92" t="n">
-        <v>0.999</v>
+        <v>0.9986945169712794</v>
       </c>
       <c r="G92" s="2" t="n">
         <v>45328.75138888889</v>
@@ -4448,10 +4448,10 @@
         <v>1165</v>
       </c>
       <c r="E93" t="n">
-        <v>6.377</v>
+        <v>6.377142857142857</v>
       </c>
       <c r="F93" t="n">
-        <v>0.958</v>
+        <v>0.95793991416309</v>
       </c>
       <c r="G93" s="2" t="n">
         <v>45329.25902777778</v>
@@ -4473,10 +4473,10 @@
         <v>2779</v>
       </c>
       <c r="E94" t="n">
-        <v>6.425</v>
+        <v>6.424691358024691</v>
       </c>
       <c r="F94" t="n">
-        <v>0.9360000000000001</v>
+        <v>0.9363080244692336</v>
       </c>
       <c r="G94" s="2" t="n">
         <v>45332.41388888889</v>
@@ -4498,10 +4498,10 @@
         <v>2057</v>
       </c>
       <c r="E95" t="n">
-        <v>6.141</v>
+        <v>6.140718562874252</v>
       </c>
       <c r="F95" t="n">
-        <v>0.997</v>
+        <v>0.9970831307729704</v>
       </c>
       <c r="G95" s="2" t="n">
         <v>45332.82638888889</v>
@@ -4523,10 +4523,10 @@
         <v>2024</v>
       </c>
       <c r="E96" t="n">
-        <v>6.171</v>
+        <v>6.17125382262997</v>
       </c>
       <c r="F96" t="n">
-        <v>0.997</v>
+        <v>0.9970355731225296</v>
       </c>
       <c r="G96" s="2" t="n">
         <v>45334.53194444445</v>
@@ -4548,10 +4548,10 @@
         <v>4037</v>
       </c>
       <c r="E97" t="n">
-        <v>6.388</v>
+        <v>6.388272583201268</v>
       </c>
       <c r="F97" t="n">
-        <v>0.999</v>
+        <v>0.9985137478325488</v>
       </c>
       <c r="G97" s="2" t="n">
         <v>45334.54027777778</v>
@@ -4573,10 +4573,10 @@
         <v>6847</v>
       </c>
       <c r="E98" t="n">
-        <v>6.058</v>
+        <v>6.057624113475177</v>
       </c>
       <c r="F98" t="n">
-        <v>0.998</v>
+        <v>0.9979553088944064</v>
       </c>
       <c r="G98" s="2" t="n">
         <v>45334.73819444444</v>
@@ -4598,10 +4598,10 @@
         <v>3519</v>
       </c>
       <c r="E99" t="n">
-        <v>5.567</v>
+        <v>5.567353407290016</v>
       </c>
       <c r="F99" t="n">
-        <v>0.998</v>
+        <v>0.998294970161978</v>
       </c>
       <c r="G99" s="2" t="n">
         <v>45334.78263888889</v>
@@ -4623,10 +4623,10 @@
         <v>3993</v>
       </c>
       <c r="E100" t="n">
-        <v>6.299</v>
+        <v>6.298578199052133</v>
       </c>
       <c r="F100" t="n">
-        <v>0.998</v>
+        <v>0.9984973703981967</v>
       </c>
       <c r="G100" s="2" t="n">
         <v>45339.73958333334</v>
@@ -4648,10 +4648,10 @@
         <v>1477</v>
       </c>
       <c r="E101" t="n">
-        <v>6.207</v>
+        <v>6.207207207207207</v>
       </c>
       <c r="F101" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.932972241029113</v>
       </c>
       <c r="G101" s="2" t="n">
         <v>45334.69791666666</v>
@@ -4673,10 +4673,10 @@
         <v>2250</v>
       </c>
       <c r="E102" t="n">
-        <v>6.275</v>
+        <v>6.274509803921569</v>
       </c>
       <c r="F102" t="n">
-        <v>0.996</v>
+        <v>0.9955555555555556</v>
       </c>
       <c r="G102" s="2" t="n">
         <v>45339.53888888889</v>
@@ -4698,10 +4698,10 @@
         <v>1485</v>
       </c>
       <c r="E103" t="n">
-        <v>5.94</v>
+        <v>5.939759036144578</v>
       </c>
       <c r="F103" t="n">
-        <v>0.996</v>
+        <v>0.995959595959596</v>
       </c>
       <c r="G103" s="2" t="n">
         <v>45339.85416666666</v>
@@ -4723,10 +4723,10 @@
         <v>1418</v>
       </c>
       <c r="E104" t="n">
-        <v>5.859</v>
+        <v>5.858921161825726</v>
       </c>
       <c r="F104" t="n">
-        <v>0.996</v>
+        <v>0.995768688293371</v>
       </c>
       <c r="G104" s="2" t="n">
         <v>45341.74027777778</v>
@@ -4748,10 +4748,10 @@
         <v>1653</v>
       </c>
       <c r="E105" t="n">
-        <v>5.967</v>
+        <v>5.967391304347826</v>
       </c>
       <c r="F105" t="n">
-        <v>0.996</v>
+        <v>0.9963702359346642</v>
       </c>
       <c r="G105" s="2" t="n">
         <v>45341.79166666666</v>
@@ -4773,10 +4773,10 @@
         <v>1281</v>
       </c>
       <c r="E106" t="n">
-        <v>5.849</v>
+        <v>5.848623853211009</v>
       </c>
       <c r="F106" t="n">
-        <v>0.995</v>
+        <v>0.9953161592505856</v>
       </c>
       <c r="G106" s="2" t="n">
         <v>45343.60416666666</v>
@@ -4798,10 +4798,10 @@
         <v>3339</v>
       </c>
       <c r="E107" t="n">
-        <v>5.766</v>
+        <v>5.76643598615917</v>
       </c>
       <c r="F107" t="n">
-        <v>0.998</v>
+        <v>0.9982030548068284</v>
       </c>
       <c r="G107" s="2" t="n">
         <v>45343.74097222222</v>
@@ -4823,10 +4823,10 @@
         <v>6379</v>
       </c>
       <c r="E108" t="n">
-        <v>6.012</v>
+        <v>6.012264150943397</v>
       </c>
       <c r="F108" t="n">
-        <v>0.999</v>
+        <v>0.9990594137012072</v>
       </c>
       <c r="G108" s="2" t="n">
         <v>45349.64097222222</v>
@@ -4848,10 +4848,10 @@
         <v>1161</v>
       </c>
       <c r="E109" t="n">
-        <v>6.243</v>
+        <v>6.243243243243243</v>
       </c>
       <c r="F109" t="n">
-        <v>0.995</v>
+        <v>0.9948320413436692</v>
       </c>
       <c r="G109" s="2" t="n">
         <v>45352.67708333334</v>
@@ -4873,10 +4873,10 @@
         <v>1933</v>
       </c>
       <c r="E110" t="n">
-        <v>6.073</v>
+        <v>6.072784810126582</v>
       </c>
       <c r="F110" t="n">
-        <v>0.993</v>
+        <v>0.9927573719606828</v>
       </c>
       <c r="G110" s="2" t="n">
         <v>45352.67708333334</v>
@@ -4898,10 +4898,10 @@
         <v>3089</v>
       </c>
       <c r="E111" t="n">
-        <v>6.423</v>
+        <v>6.422916666666667</v>
       </c>
       <c r="F111" t="n">
-        <v>0.998</v>
+        <v>0.9980576238264812</v>
       </c>
       <c r="G111" s="2" t="n">
         <v>45353.81111111111</v>
@@ -4923,10 +4923,10 @@
         <v>1929</v>
       </c>
       <c r="E112" t="n">
-        <v>6.475</v>
+        <v>6.474747474747475</v>
       </c>
       <c r="F112" t="n">
-        <v>0.997</v>
+        <v>0.9968895800933126</v>
       </c>
       <c r="G112" s="2" t="n">
         <v>45353.82013888889</v>
@@ -4948,10 +4948,10 @@
         <v>8292</v>
       </c>
       <c r="E113" t="n">
-        <v>5.951</v>
+        <v>5.950617283950617</v>
       </c>
       <c r="F113" t="n">
-        <v>0.988</v>
+        <v>0.9881813796430294</v>
       </c>
       <c r="G113" s="2" t="n">
         <v>45351.75972222222</v>
@@ -4973,10 +4973,10 @@
         <v>2781</v>
       </c>
       <c r="E114" t="n">
-        <v>5.946</v>
+        <v>5.94553376906318</v>
       </c>
       <c r="F114" t="n">
-        <v>0.981</v>
+        <v>0.981301690039554</v>
       </c>
       <c r="G114" s="2" t="n">
         <v>45357.76388888889</v>
@@ -4998,10 +4998,10 @@
         <v>1415</v>
       </c>
       <c r="E115" t="n">
-        <v>5.833</v>
+        <v>5.833333333333333</v>
       </c>
       <c r="F115" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.939929328621908</v>
       </c>
       <c r="G115" s="2" t="n">
         <v>45359.66180555556</v>
@@ -5023,10 +5023,10 @@
         <v>1293</v>
       </c>
       <c r="E116" t="n">
-        <v>5.83</v>
+        <v>5.830275229357798</v>
       </c>
       <c r="F116" t="n">
-        <v>0.983</v>
+        <v>0.982985305491106</v>
       </c>
       <c r="G116" s="2" t="n">
         <v>45362.80833333333</v>
@@ -5048,10 +5048,10 @@
         <v>2800</v>
       </c>
       <c r="E117" t="n">
-        <v>6.423</v>
+        <v>6.422988505747126</v>
       </c>
       <c r="F117" t="n">
-        <v>0.998</v>
+        <v>0.9978571428571428</v>
       </c>
       <c r="G117" s="2" t="n">
         <v>45364.67430555556</v>
@@ -5073,10 +5073,10 @@
         <v>2251</v>
       </c>
       <c r="E118" t="n">
-        <v>5.877</v>
+        <v>5.87696335078534</v>
       </c>
       <c r="F118" t="n">
-        <v>0.997</v>
+        <v>0.9973345179920036</v>
       </c>
       <c r="G118" s="2" t="n">
         <v>45363.69305555556</v>
@@ -5098,10 +5098,10 @@
         <v>9050</v>
       </c>
       <c r="E119" t="n">
-        <v>6.121</v>
+        <v>6.120514556533514</v>
       </c>
       <c r="F119" t="n">
-        <v>0.999</v>
+        <v>0.9988950276243094</v>
       </c>
       <c r="G119" s="2" t="n">
         <v>45585.69652777778</v>
@@ -5123,10 +5123,10 @@
         <v>3444</v>
       </c>
       <c r="E120" t="n">
-        <v>5.99</v>
+        <v>5.989547038327526</v>
       </c>
       <c r="F120" t="n">
-        <v>0.998</v>
+        <v>0.9982578397212544</v>
       </c>
       <c r="G120" s="2" t="n">
         <v>45364.67222222222</v>
@@ -5148,10 +5148,10 @@
         <v>8626</v>
       </c>
       <c r="E121" t="n">
-        <v>6.306</v>
+        <v>6.305779078273591</v>
       </c>
       <c r="F121" t="n">
-        <v>0.999</v>
+        <v>0.9993044284720612</v>
       </c>
       <c r="G121" s="2" t="n">
         <v>45366.76041666666</v>
@@ -5173,10 +5173,10 @@
         <v>3592</v>
       </c>
       <c r="E122" t="n">
-        <v>6.237</v>
+        <v>6.236521739130435</v>
       </c>
       <c r="F122" t="n">
-        <v>0.998</v>
+        <v>0.9983296213808464</v>
       </c>
       <c r="G122" s="2" t="n">
         <v>45370.75208333333</v>
@@ -5198,10 +5198,10 @@
         <v>15229</v>
       </c>
       <c r="E123" t="n">
-        <v>6.295</v>
+        <v>6.295369211514393</v>
       </c>
       <c r="F123" t="n">
-        <v>0.991</v>
+        <v>0.9908726771291616</v>
       </c>
       <c r="G123" s="2" t="n">
         <v>45374.78958333333</v>
@@ -5223,10 +5223,10 @@
         <v>2723</v>
       </c>
       <c r="E124" t="n">
-        <v>6.217</v>
+        <v>6.217391304347826</v>
       </c>
       <c r="F124" t="n">
-        <v>0.998</v>
+        <v>0.9977965479250828</v>
       </c>
       <c r="G124" s="2" t="n">
         <v>45375.90555555555</v>
@@ -5248,10 +5248,10 @@
         <v>4358</v>
       </c>
       <c r="E125" t="n">
-        <v>6.509</v>
+        <v>6.50920245398773</v>
       </c>
       <c r="F125" t="n">
-        <v>0.974</v>
+        <v>0.973841211564938</v>
       </c>
       <c r="G125" s="2" t="n">
         <v>45376.37638888889</v>
@@ -5273,10 +5273,10 @@
         <v>1654</v>
       </c>
       <c r="E126" t="n">
-        <v>6.645</v>
+        <v>6.645161290322581</v>
       </c>
       <c r="F126" t="n">
-        <v>0.996</v>
+        <v>0.996372430471584</v>
       </c>
       <c r="G126" s="2" t="n">
         <v>45376.42152777778</v>
@@ -5298,10 +5298,10 @@
         <v>4595</v>
       </c>
       <c r="E127" t="n">
-        <v>5.997</v>
+        <v>5.997371879106439</v>
       </c>
       <c r="F127" t="n">
-        <v>0.993</v>
+        <v>0.993253536452666</v>
       </c>
       <c r="G127" s="2" t="n">
         <v>45376.7625</v>
@@ -5323,10 +5323,10 @@
         <v>805</v>
       </c>
       <c r="E128" t="n">
-        <v>5.963</v>
+        <v>5.962686567164179</v>
       </c>
       <c r="F128" t="n">
-        <v>0.993</v>
+        <v>0.9925465838509316</v>
       </c>
       <c r="G128" s="2" t="n">
         <v>45376.78333333333</v>
@@ -5348,10 +5348,10 @@
         <v>887</v>
       </c>
       <c r="E129" t="n">
-        <v>5.721</v>
+        <v>5.720779220779221</v>
       </c>
       <c r="F129" t="n">
-        <v>0.993</v>
+        <v>0.9932356257046224</v>
       </c>
       <c r="G129" s="2" t="n">
         <v>45376.78333333333</v>
@@ -5373,10 +5373,10 @@
         <v>2157</v>
       </c>
       <c r="E130" t="n">
-        <v>6.303</v>
+        <v>6.302941176470588</v>
       </c>
       <c r="F130" t="n">
-        <v>0.994</v>
+        <v>0.9935095039406584</v>
       </c>
       <c r="G130" s="2" t="n">
         <v>45378.78402777778</v>
@@ -5398,10 +5398,10 @@
         <v>1994</v>
       </c>
       <c r="E131" t="n">
-        <v>6.479</v>
+        <v>6.478547854785479</v>
       </c>
       <c r="F131" t="n">
-        <v>0.984</v>
+        <v>0.9844533600802408</v>
       </c>
       <c r="G131" s="2" t="n">
         <v>45385.35902777778</v>
@@ -5423,10 +5423,10 @@
         <v>2459</v>
       </c>
       <c r="E132" t="n">
-        <v>6.594</v>
+        <v>6.594086021505376</v>
       </c>
       <c r="F132" t="n">
-        <v>0.998</v>
+        <v>0.9975599837332249</v>
       </c>
       <c r="G132" s="2" t="n">
         <v>45386.84583333333</v>
@@ -5448,10 +5448,10 @@
         <v>2130</v>
       </c>
       <c r="E133" t="n">
-        <v>6.157</v>
+        <v>6.156521739130435</v>
       </c>
       <c r="F133" t="n">
-        <v>0.997</v>
+        <v>0.9971830985915492</v>
       </c>
       <c r="G133" s="2" t="n">
         <v>45387.43055555555</v>
@@ -5473,10 +5473,10 @@
         <v>8210</v>
       </c>
       <c r="E134" t="n">
-        <v>5.965</v>
+        <v>5.964963503649635</v>
       </c>
       <c r="F134" t="n">
-        <v>0.995</v>
+        <v>0.9953714981729598</v>
       </c>
       <c r="G134" s="2" t="n">
         <v>45390.84513888889</v>
@@ -5498,10 +5498,10 @@
         <v>4751</v>
       </c>
       <c r="E135" t="n">
-        <v>6.091</v>
+        <v>6.091142490372272</v>
       </c>
       <c r="F135" t="n">
-        <v>0.999</v>
+        <v>0.998737107977268</v>
       </c>
       <c r="G135" s="2" t="n">
         <v>45391.81388888889</v>
@@ -5523,10 +5523,10 @@
         <v>1533</v>
       </c>
       <c r="E136" t="n">
-        <v>6.233</v>
+        <v>6.232653061224489</v>
       </c>
       <c r="F136" t="n">
-        <v>0.996</v>
+        <v>0.9960861056751468</v>
       </c>
       <c r="G136" s="2" t="n">
         <v>45394.68333333333</v>
@@ -5548,10 +5548,10 @@
         <v>3465</v>
       </c>
       <c r="E137" t="n">
-        <v>6.019</v>
+        <v>6.019400352733686</v>
       </c>
       <c r="F137" t="n">
-        <v>0.985</v>
+        <v>0.984992784992785</v>
       </c>
       <c r="G137" s="2" t="n">
         <v>45394.81458333333</v>
@@ -5573,10 +5573,10 @@
         <v>1302</v>
       </c>
       <c r="E138" t="n">
-        <v>5.812</v>
+        <v>5.811659192825112</v>
       </c>
       <c r="F138" t="n">
-        <v>0.995</v>
+        <v>0.9953917050691244</v>
       </c>
       <c r="G138" s="2" t="n">
         <v>45396.38402777778</v>
@@ -5598,10 +5598,10 @@
         <v>2031</v>
       </c>
       <c r="E139" t="n">
-        <v>6.269</v>
+        <v>6.269349845201238</v>
       </c>
       <c r="F139" t="n">
-        <v>0.997</v>
+        <v>0.9970457902511078</v>
       </c>
       <c r="G139" s="2" t="n">
         <v>45398.74375</v>
@@ -5623,10 +5623,10 @@
         <v>1552</v>
       </c>
       <c r="E140" t="n">
-        <v>6.496</v>
+        <v>6.495798319327731</v>
       </c>
       <c r="F140" t="n">
-        <v>0.996</v>
+        <v>0.9961340206185568</v>
       </c>
       <c r="G140" s="2" t="n">
         <v>45398.76180555556</v>
@@ -5648,10 +5648,10 @@
         <v>1921</v>
       </c>
       <c r="E141" t="n">
-        <v>6.14</v>
+        <v>6.13961038961039</v>
       </c>
       <c r="F141" t="n">
-        <v>0.984</v>
+        <v>0.9843831337844872</v>
       </c>
       <c r="G141" s="2" t="n">
         <v>45403.59305555555</v>
@@ -5673,10 +5673,10 @@
         <v>1942</v>
       </c>
       <c r="E142" t="n">
-        <v>6.306</v>
+        <v>6.306188925081433</v>
       </c>
       <c r="F142" t="n">
-        <v>0.997</v>
+        <v>0.9969104016477858</v>
       </c>
       <c r="G142" s="2" t="n">
         <v>45403.83888888889</v>
@@ -5698,10 +5698,10 @@
         <v>1516</v>
       </c>
       <c r="E143" t="n">
-        <v>6.648</v>
+        <v>6.648401826484018</v>
       </c>
       <c r="F143" t="n">
-        <v>0.96</v>
+        <v>0.9604221635883904</v>
       </c>
       <c r="G143" s="2" t="n">
         <v>45406.61180555556</v>
@@ -5723,10 +5723,10 @@
         <v>1271</v>
       </c>
       <c r="E144" t="n">
-        <v>6.765</v>
+        <v>6.764705882352941</v>
       </c>
       <c r="F144" t="n">
-        <v>0.995</v>
+        <v>0.995279307631786</v>
       </c>
       <c r="G144" s="2" t="n">
         <v>45407.59791666667</v>
@@ -5748,10 +5748,10 @@
         <v>1403</v>
       </c>
       <c r="E145" t="n">
-        <v>6.332</v>
+        <v>6.331818181818182</v>
       </c>
       <c r="F145" t="n">
-        <v>0.993</v>
+        <v>0.992872416250891</v>
       </c>
       <c r="G145" s="2" t="n">
         <v>45419.78611111111</v>
@@ -5773,10 +5773,10 @@
         <v>1829</v>
       </c>
       <c r="E146" t="n">
-        <v>6.222</v>
+        <v>6.221843003412969</v>
       </c>
       <c r="F146" t="n">
-        <v>0.997</v>
+        <v>0.9967195188627666</v>
       </c>
       <c r="G146" s="2" t="n">
         <v>45423.75902777778</v>
@@ -5798,10 +5798,10 @@
         <v>4478</v>
       </c>
       <c r="E147" t="n">
-        <v>6.352</v>
+        <v>6.352272727272728</v>
       </c>
       <c r="F147" t="n">
-        <v>0.999</v>
+        <v>0.9986601161232692</v>
       </c>
       <c r="G147" s="2" t="n">
         <v>45424.53333333333</v>
@@ -5823,10 +5823,10 @@
         <v>7774</v>
       </c>
       <c r="E148" t="n">
-        <v>6.404</v>
+        <v>6.403957131079968</v>
       </c>
       <c r="F148" t="n">
-        <v>0.999</v>
+        <v>0.9992281965526112</v>
       </c>
       <c r="G148" s="2" t="n">
         <v>45424.75069444445</v>
@@ -5848,10 +5848,10 @@
         <v>4301</v>
       </c>
       <c r="E149" t="n">
-        <v>7.17</v>
+        <v>7.170283806343907</v>
       </c>
       <c r="F149" t="n">
-        <v>0.999</v>
+        <v>0.9986049755870728</v>
       </c>
       <c r="G149" s="2" t="n">
         <v>45427.36944444444</v>
@@ -5873,10 +5873,10 @@
         <v>3524</v>
       </c>
       <c r="E150" t="n">
-        <v>6.194</v>
+        <v>6.193661971830986</v>
       </c>
       <c r="F150" t="n">
-        <v>0.998</v>
+        <v>0.9982973893303064</v>
       </c>
       <c r="G150" s="2" t="n">
         <v>45432.49444444444</v>
@@ -5898,10 +5898,10 @@
         <v>1788</v>
       </c>
       <c r="E151" t="n">
-        <v>6.166</v>
+        <v>6.166089965397924</v>
       </c>
       <c r="F151" t="n">
-        <v>0.997</v>
+        <v>0.9966442953020134</v>
       </c>
       <c r="G151" s="2" t="n">
         <v>45433.69444444445</v>
@@ -5923,10 +5923,10 @@
         <v>15749</v>
       </c>
       <c r="E152" t="n">
-        <v>6.276</v>
+        <v>6.275931117340809</v>
       </c>
       <c r="F152" t="n">
-        <v>0.995</v>
+        <v>0.9950473045907676</v>
       </c>
       <c r="G152" s="2" t="n">
         <v>45441.75069444445</v>
@@ -5948,10 +5948,10 @@
         <v>2741</v>
       </c>
       <c r="E153" t="n">
-        <v>5.806</v>
+        <v>5.805970149253731</v>
       </c>
       <c r="F153" t="n">
-        <v>0.993</v>
+        <v>0.993433053630062</v>
       </c>
       <c r="G153" s="2" t="n">
         <v>45443.51041666666</v>
@@ -5973,10 +5973,10 @@
         <v>1638</v>
       </c>
       <c r="E154" t="n">
-        <v>6.205</v>
+        <v>6.20532319391635</v>
       </c>
       <c r="F154" t="n">
-        <v>0.996</v>
+        <v>0.9963369963369964</v>
       </c>
       <c r="G154" s="2" t="n">
         <v>45444.70763888889</v>
@@ -5998,10 +5998,10 @@
         <v>1652</v>
       </c>
       <c r="E155" t="n">
-        <v>6.235</v>
+        <v>6.234848484848484</v>
       </c>
       <c r="F155" t="n">
-        <v>0.996</v>
+        <v>0.9963680387409199</v>
       </c>
       <c r="G155" s="2" t="n">
         <v>45454.77569444444</v>
@@ -6023,10 +6023,10 @@
         <v>4211</v>
       </c>
       <c r="E156" t="n">
-        <v>6.342</v>
+        <v>6.342383107088989</v>
       </c>
       <c r="F156" t="n">
-        <v>0.999</v>
+        <v>0.9985751602944668</v>
       </c>
       <c r="G156" s="2" t="n">
         <v>45453.66041666667</v>
@@ -6048,10 +6048,10 @@
         <v>8760</v>
       </c>
       <c r="E157" t="n">
-        <v>6.234</v>
+        <v>6.23445318084346</v>
       </c>
       <c r="F157" t="n">
-        <v>0.996</v>
+        <v>0.995662100456621</v>
       </c>
       <c r="G157" s="2" t="n">
         <v>45455.64583333334</v>
@@ -6073,10 +6073,10 @@
         <v>2500</v>
       </c>
       <c r="E158" t="n">
-        <v>6.362</v>
+        <v>6.362244897959184</v>
       </c>
       <c r="F158" t="n">
-        <v>0.998</v>
+        <v>0.9976</v>
       </c>
       <c r="G158" s="2" t="n">
         <v>45458.84097222222</v>
@@ -6098,10 +6098,10 @@
         <v>5104</v>
       </c>
       <c r="E159" t="n">
-        <v>6.019</v>
+        <v>6.018890200708382</v>
       </c>
       <c r="F159" t="n">
-        <v>0.999</v>
+        <v>0.9988244514106585</v>
       </c>
       <c r="G159" s="2" t="n">
         <v>45465.41805555556</v>
@@ -6123,10 +6123,10 @@
         <v>1571</v>
       </c>
       <c r="E160" t="n">
-        <v>6.186</v>
+        <v>6.185770750988143</v>
       </c>
       <c r="F160" t="n">
-        <v>0.996</v>
+        <v>0.9961807765754296</v>
       </c>
       <c r="G160" s="2" t="n">
         <v>45466.83194444444</v>
@@ -6148,10 +6148,10 @@
         <v>3913</v>
       </c>
       <c r="E161" t="n">
-        <v>6.374</v>
+        <v>6.373572593800978</v>
       </c>
       <c r="F161" t="n">
-        <v>0.998</v>
+        <v>0.9984666496294404</v>
       </c>
       <c r="G161" s="2" t="n">
         <v>45467.65486111111</v>
@@ -6173,10 +6173,10 @@
         <v>4328</v>
       </c>
       <c r="E162" t="n">
-        <v>6.174</v>
+        <v>6.174285714285714</v>
       </c>
       <c r="F162" t="n">
-        <v>0.999</v>
+        <v>0.9986136783733828</v>
       </c>
       <c r="G162" s="2" t="n">
         <v>45468.69027777778</v>
@@ -6198,10 +6198,10 @@
         <v>1693</v>
       </c>
       <c r="E163" t="n">
-        <v>6.271</v>
+        <v>6.271375464684015</v>
       </c>
       <c r="F163" t="n">
-        <v>0.996</v>
+        <v>0.9964559952746604</v>
       </c>
       <c r="G163" s="2" t="n">
         <v>45472.69236111111</v>
@@ -6223,10 +6223,10 @@
         <v>5942</v>
       </c>
       <c r="E164" t="n">
-        <v>6.151</v>
+        <v>6.151295336787565</v>
       </c>
       <c r="F164" t="n">
-        <v>0.999</v>
+        <v>0.9989902389767756</v>
       </c>
       <c r="G164" s="2" t="n">
         <v>45473.78611111111</v>
@@ -6248,10 +6248,10 @@
         <v>10527</v>
       </c>
       <c r="E165" t="n">
-        <v>6.187</v>
+        <v>6.186721991701245</v>
       </c>
       <c r="F165" t="n">
-        <v>0.991</v>
+        <v>0.9914505557138786</v>
       </c>
       <c r="G165" s="2" t="n">
         <v>45475.65972222222</v>
@@ -6273,10 +6273,10 @@
         <v>1729</v>
       </c>
       <c r="E166" t="n">
-        <v>6.837</v>
+        <v>6.837301587301587</v>
       </c>
       <c r="F166" t="n">
-        <v>0.997</v>
+        <v>0.9965297860034702</v>
       </c>
       <c r="G166" s="2" t="n">
         <v>45476.67291666667</v>
@@ -6298,10 +6298,10 @@
         <v>10321</v>
       </c>
       <c r="E167" t="n">
-        <v>6.336</v>
+        <v>6.335995085995086</v>
       </c>
       <c r="F167" t="n">
-        <v>0.999</v>
+        <v>0.9994186609824628</v>
       </c>
       <c r="G167" s="2" t="n">
         <v>45484.85694444444</v>
@@ -6323,10 +6323,10 @@
         <v>4065</v>
       </c>
       <c r="E168" t="n">
-        <v>6.412</v>
+        <v>6.412322274881516</v>
       </c>
       <c r="F168" t="n">
-        <v>0.999</v>
+        <v>0.9985239852398524</v>
       </c>
       <c r="G168" s="2" t="n">
         <v>45486.65902777778</v>
@@ -6348,10 +6348,10 @@
         <v>3820</v>
       </c>
       <c r="E169" t="n">
-        <v>5.997</v>
+        <v>5.99685534591195</v>
       </c>
       <c r="F169" t="n">
-        <v>0.998</v>
+        <v>0.9984293193717276</v>
       </c>
       <c r="G169" s="2" t="n">
         <v>45490.67986111111</v>
@@ -6373,10 +6373,10 @@
         <v>7712</v>
       </c>
       <c r="E170" t="n">
-        <v>6.275</v>
+        <v>6.275244299674267</v>
       </c>
       <c r="F170" t="n">
-        <v>0.999</v>
+        <v>0.9992219917012448</v>
       </c>
       <c r="G170" s="2" t="n">
         <v>45492.65555555555</v>
@@ -6398,10 +6398,10 @@
         <v>4008</v>
       </c>
       <c r="E171" t="n">
-        <v>6.617</v>
+        <v>6.616915422885572</v>
       </c>
       <c r="F171" t="n">
-        <v>0.996</v>
+        <v>0.9955089820359282</v>
       </c>
       <c r="G171" s="2" t="n">
         <v>45494.78055555555</v>
@@ -6423,10 +6423,10 @@
         <v>32846</v>
       </c>
       <c r="E172" t="n">
-        <v>6.415</v>
+        <v>6.414548298787642</v>
       </c>
       <c r="F172" t="n">
-        <v>0.999</v>
+        <v>0.9987213054862084</v>
       </c>
       <c r="G172" s="2" t="n">
         <v>45494.80833333333</v>
@@ -6448,10 +6448,10 @@
         <v>9027</v>
       </c>
       <c r="E173" t="n">
-        <v>6.106</v>
+        <v>6.106027596223675</v>
       </c>
       <c r="F173" t="n">
-        <v>0.931</v>
+        <v>0.9314279384070012</v>
       </c>
       <c r="G173" s="2" t="n">
         <v>45496.71944444445</v>
@@ -6473,10 +6473,10 @@
         <v>7615</v>
       </c>
       <c r="E174" t="n">
-        <v>6.332</v>
+        <v>6.332223147377186</v>
       </c>
       <c r="F174" t="n">
-        <v>0.999</v>
+        <v>0.9986868023637556</v>
       </c>
       <c r="G174" s="2" t="n">
         <v>45506.79236111111</v>
@@ -6498,10 +6498,10 @@
         <v>7692</v>
       </c>
       <c r="E175" t="n">
-        <v>6.336</v>
+        <v>6.336356141797197</v>
       </c>
       <c r="F175" t="n">
-        <v>0.999</v>
+        <v>0.999219968798752</v>
       </c>
       <c r="G175" s="2" t="n">
         <v>45507.64444444444</v>
@@ -6523,10 +6523,10 @@
         <v>8880</v>
       </c>
       <c r="E176" t="n">
-        <v>6.078</v>
+        <v>6.078082191780822</v>
       </c>
       <c r="F176" t="n">
-        <v>0.999</v>
+        <v>0.9993243243243244</v>
       </c>
       <c r="G176" s="2" t="n">
         <v>45515.73611111111</v>
@@ -6548,10 +6548,10 @@
         <v>2374</v>
       </c>
       <c r="E177" t="n">
-        <v>6.505</v>
+        <v>6.505494505494505</v>
       </c>
       <c r="F177" t="n">
-        <v>0.997</v>
+        <v>0.9974726200505476</v>
       </c>
       <c r="G177" s="2" t="n">
         <v>45520.62847222222</v>
@@ -6573,10 +6573,10 @@
         <v>4496</v>
       </c>
       <c r="E178" t="n">
-        <v>6.28</v>
+        <v>6.27972027972028</v>
       </c>
       <c r="F178" t="n">
-        <v>0.999</v>
+        <v>0.9986654804270464</v>
       </c>
       <c r="G178" s="2" t="n">
         <v>45540.28541666667</v>
@@ -6598,10 +6598,10 @@
         <v>2071</v>
       </c>
       <c r="E179" t="n">
-        <v>5.934</v>
+        <v>5.933908045977011</v>
       </c>
       <c r="F179" t="n">
-        <v>0.997</v>
+        <v>0.9971028488652824</v>
       </c>
       <c r="G179" s="2" t="n">
         <v>45544.62777777778</v>
@@ -6623,10 +6623,10 @@
         <v>9176</v>
       </c>
       <c r="E180" t="n">
-        <v>6.498</v>
+        <v>6.497872340425532</v>
       </c>
       <c r="F180" t="n">
-        <v>0.998</v>
+        <v>0.9984742807323452</v>
       </c>
       <c r="G180" s="2" t="n">
         <v>45545.69027777778</v>
@@ -6648,10 +6648,10 @@
         <v>3768</v>
       </c>
       <c r="E181" t="n">
-        <v>6.111</v>
+        <v>6.110569105691057</v>
       </c>
       <c r="F181" t="n">
-        <v>0.997</v>
+        <v>0.9973460721868364</v>
       </c>
       <c r="G181" s="2" t="n">
         <v>45547.78472222222</v>
@@ -6673,10 +6673,10 @@
         <v>2331</v>
       </c>
       <c r="E182" t="n">
-        <v>6.039</v>
+        <v>6.038961038961039</v>
       </c>
       <c r="F182" t="n">
-        <v>0.997</v>
+        <v>0.9974259974259976</v>
       </c>
       <c r="G182" s="2" t="n">
         <v>45548.69513888889</v>
@@ -6698,10 +6698,10 @@
         <v>7423</v>
       </c>
       <c r="E183" t="n">
-        <v>6.489</v>
+        <v>6.489063867016623</v>
       </c>
       <c r="F183" t="n">
-        <v>0.999</v>
+        <v>0.999191701468409</v>
       </c>
       <c r="G183" s="2" t="n">
         <v>45556.69722222222</v>
@@ -6723,10 +6723,10 @@
         <v>5060</v>
       </c>
       <c r="E184" t="n">
-        <v>6.471</v>
+        <v>6.471190781049936</v>
       </c>
       <c r="F184" t="n">
-        <v>0.999</v>
+        <v>0.998814229249012</v>
       </c>
       <c r="G184" s="2" t="n">
         <v>45553.69513888889</v>
@@ -6748,10 +6748,10 @@
         <v>4417</v>
       </c>
       <c r="E185" t="n">
-        <v>6.525</v>
+        <v>6.525147928994083</v>
       </c>
       <c r="F185" t="n">
-        <v>0.999</v>
+        <v>0.9986416119538148</v>
       </c>
       <c r="G185" s="2" t="n">
         <v>45565.76458333333</v>
@@ -6773,10 +6773,10 @@
         <v>11417</v>
       </c>
       <c r="E186" t="n">
-        <v>6.329</v>
+        <v>6.328843995510662</v>
       </c>
       <c r="F186" t="n">
-        <v>0.988</v>
+        <v>0.98782517298765</v>
       </c>
       <c r="G186" s="2" t="n">
         <v>45568.53333333333</v>
@@ -6798,10 +6798,10 @@
         <v>1964</v>
       </c>
       <c r="E187" t="n">
-        <v>6.257</v>
+        <v>6.257234726688103</v>
       </c>
       <c r="F187" t="n">
-        <v>0.991</v>
+        <v>0.9908350305498982</v>
       </c>
       <c r="G187" s="2" t="n">
         <v>45569.63958333333</v>
@@ -6823,10 +6823,10 @@
         <v>3181</v>
       </c>
       <c r="E188" t="n">
-        <v>6.317</v>
+        <v>6.316733067729084</v>
       </c>
       <c r="F188" t="n">
-        <v>0.997</v>
+        <v>0.9968563344860109</v>
       </c>
       <c r="G188" s="2" t="n">
         <v>45569.77222222222</v>
@@ -6848,10 +6848,10 @@
         <v>1727</v>
       </c>
       <c r="E189" t="n">
-        <v>6.452</v>
+        <v>6.451737451737452</v>
       </c>
       <c r="F189" t="n">
-        <v>0.968</v>
+        <v>0.9675738274464388</v>
       </c>
       <c r="G189" s="2" t="n">
         <v>45570.81458333333</v>
@@ -6873,10 +6873,10 @@
         <v>4279</v>
       </c>
       <c r="E190" t="n">
-        <v>6.14</v>
+        <v>6.139769452449568</v>
       </c>
       <c r="F190" t="n">
-        <v>0.996</v>
+        <v>0.9957934096751576</v>
       </c>
       <c r="G190" s="2" t="n">
         <v>45571.66319444445</v>
@@ -6898,10 +6898,10 @@
         <v>4463</v>
       </c>
       <c r="E191" t="n">
-        <v>6.339</v>
+        <v>6.339080459770115</v>
       </c>
       <c r="F191" t="n">
-        <v>0.989</v>
+        <v>0.9885727089401748</v>
       </c>
       <c r="G191" s="2" t="n">
         <v>45574.7</v>
@@ -6923,10 +6923,10 @@
         <v>6654</v>
       </c>
       <c r="E192" t="n">
-        <v>6.52</v>
+        <v>6.520117762512267</v>
       </c>
       <c r="F192" t="n">
-        <v>0.998</v>
+        <v>0.998497144574692</v>
       </c>
       <c r="G192" s="2" t="n">
         <v>45575.65</v>
@@ -6948,10 +6948,10 @@
         <v>3366</v>
       </c>
       <c r="E193" t="n">
-        <v>6.165</v>
+        <v>6.165137614678899</v>
       </c>
       <c r="F193" t="n">
-        <v>0.998</v>
+        <v>0.9982174688057039</v>
       </c>
       <c r="G193" s="2" t="n">
         <v>45575.79513888889</v>
@@ -6973,10 +6973,10 @@
         <v>4519</v>
       </c>
       <c r="E194" t="n">
-        <v>6.56</v>
+        <v>6.559593023255814</v>
       </c>
       <c r="F194" t="n">
-        <v>0.999</v>
+        <v>0.9986722726266872</v>
       </c>
       <c r="G194" s="2" t="n">
         <v>45576.73541666667</v>
@@ -6998,10 +6998,10 @@
         <v>9151</v>
       </c>
       <c r="E195" t="n">
-        <v>6.551</v>
+        <v>6.550859598853868</v>
       </c>
       <c r="F195" t="n">
-        <v>0.999</v>
+        <v>0.9993443339525736</v>
       </c>
       <c r="G195" s="2" t="n">
         <v>45582.68888888889</v>
@@ -7023,10 +7023,10 @@
         <v>6229</v>
       </c>
       <c r="E196" t="n">
-        <v>6.344</v>
+        <v>6.343621399176954</v>
       </c>
       <c r="F196" t="n">
-        <v>0.99</v>
+        <v>0.9898860170171776</v>
       </c>
       <c r="G196" s="2" t="n">
         <v>45583.69305555556</v>
@@ -7048,10 +7048,10 @@
         <v>3659</v>
       </c>
       <c r="E197" t="n">
-        <v>6.398</v>
+        <v>6.397548161120841</v>
       </c>
       <c r="F197" t="n">
-        <v>0.998</v>
+        <v>0.9983602077070238</v>
       </c>
       <c r="G197" s="2" t="n">
         <v>45587.70625</v>
@@ -7073,10 +7073,10 @@
         <v>4059</v>
       </c>
       <c r="E198" t="n">
-        <v>6.313</v>
+        <v>6.313084112149533</v>
       </c>
       <c r="F198" t="n">
-        <v>0.999</v>
+        <v>0.9985218033998522</v>
       </c>
       <c r="G198" s="2" t="n">
         <v>45589.74305555555</v>
@@ -7098,10 +7098,10 @@
         <v>4912</v>
       </c>
       <c r="E199" t="n">
-        <v>6.242</v>
+        <v>6.242307692307692</v>
       </c>
       <c r="F199" t="n">
-        <v>0.991</v>
+        <v>0.9912459283387622</v>
       </c>
       <c r="G199" s="2" t="n">
         <v>45592.68888888889</v>
@@ -7123,10 +7123,10 @@
         <v>3437</v>
       </c>
       <c r="E200" t="n">
-        <v>6.009</v>
+        <v>6.008756567425569</v>
       </c>
       <c r="F200" t="n">
-        <v>0.998</v>
+        <v>0.998254291533314</v>
       </c>
       <c r="G200" s="2" t="n">
         <v>45595.65277777778</v>
@@ -7148,10 +7148,10 @@
         <v>6595</v>
       </c>
       <c r="E201" t="n">
-        <v>6.228</v>
+        <v>6.227788279773157</v>
       </c>
       <c r="F201" t="n">
-        <v>0.999</v>
+        <v>0.999090219863533</v>
       </c>
       <c r="G201" s="2" t="n">
         <v>45601.76875</v>
@@ -7173,10 +7173,10 @@
         <v>3021</v>
       </c>
       <c r="E202" t="n">
-        <v>6.042</v>
+        <v>6.042084168336673</v>
       </c>
       <c r="F202" t="n">
-        <v>0.998</v>
+        <v>0.9980139026812314</v>
       </c>
       <c r="G202" s="2" t="n">
         <v>45603.725</v>
@@ -7198,10 +7198,10 @@
         <v>1801</v>
       </c>
       <c r="E203" t="n">
-        <v>6.851</v>
+        <v>6.851145038167939</v>
       </c>
       <c r="F203" t="n">
-        <v>0.997</v>
+        <v>0.9966685174902832</v>
       </c>
       <c r="G203" s="2" t="n">
         <v>45603.78888888889</v>
@@ -7223,10 +7223,10 @@
         <v>1903</v>
       </c>
       <c r="E204" t="n">
-        <v>6.727</v>
+        <v>6.726950354609929</v>
       </c>
       <c r="F204" t="n">
-        <v>0.997</v>
+        <v>0.996847083552286</v>
       </c>
       <c r="G204" s="2" t="n">
         <v>45607.76319444444</v>
@@ -7248,10 +7248,10 @@
         <v>5245</v>
       </c>
       <c r="E205" t="n">
-        <v>6.319</v>
+        <v>6.318840579710145</v>
       </c>
       <c r="F205" t="n">
-        <v>0.998</v>
+        <v>0.9975214489990468</v>
       </c>
       <c r="G205" s="2" t="n">
         <v>45608.51041666666</v>
@@ -7273,10 +7273,10 @@
         <v>2128</v>
       </c>
       <c r="E206" t="n">
-        <v>8.733000000000001</v>
+        <v>8.732510288065845</v>
       </c>
       <c r="F206" t="n">
-        <v>0.997</v>
+        <v>0.9971804511278196</v>
       </c>
       <c r="G206" s="2" t="n">
         <v>45613.76111111111</v>
@@ -7298,10 +7298,10 @@
         <v>5617</v>
       </c>
       <c r="E207" t="n">
-        <v>6.502</v>
+        <v>6.501738122827346</v>
       </c>
       <c r="F207" t="n">
-        <v>0.999</v>
+        <v>0.9989318141356596</v>
       </c>
       <c r="G207" s="2" t="n">
         <v>45616.66527777778</v>
@@ -7323,10 +7323,10 @@
         <v>3822</v>
       </c>
       <c r="E208" t="n">
-        <v>6.424</v>
+        <v>6.424242424242424</v>
       </c>
       <c r="F208" t="n">
-        <v>0.998</v>
+        <v>0.998430141287284</v>
       </c>
       <c r="G208" s="2" t="n">
         <v>45621.625</v>
@@ -7348,10 +7348,10 @@
         <v>8594</v>
       </c>
       <c r="E209" t="n">
-        <v>6.287</v>
+        <v>6.287077826725404</v>
       </c>
       <c r="F209" t="n">
-        <v>0.996</v>
+        <v>0.9963928322085176</v>
       </c>
       <c r="G209" s="2" t="n">
         <v>45621.77708333333</v>
@@ -7373,10 +7373,10 @@
         <v>3950</v>
       </c>
       <c r="E210" t="n">
-        <v>6.541</v>
+        <v>6.540630182421228</v>
       </c>
       <c r="F210" t="n">
-        <v>0.998</v>
+        <v>0.998481012658228</v>
       </c>
       <c r="G210" s="2" t="n">
         <v>45638.65138888889</v>
@@ -7398,10 +7398,10 @@
         <v>5327</v>
       </c>
       <c r="E211" t="n">
-        <v>6.561</v>
+        <v>6.561035758323058</v>
       </c>
       <c r="F211" t="n">
-        <v>0.999</v>
+        <v>0.998873662474188</v>
       </c>
       <c r="G211" s="2" t="n">
         <v>45645.69861111111</v>
@@ -7423,10 +7423,10 @@
         <v>3957</v>
       </c>
       <c r="E212" t="n">
-        <v>6.279</v>
+        <v>6.278662420382165</v>
       </c>
       <c r="F212" t="n">
-        <v>0.996</v>
+        <v>0.9964619661359616</v>
       </c>
       <c r="G212" s="2" t="n">
         <v>45675.74444444444</v>
@@ -7448,10 +7448,10 @@
         <v>4019</v>
       </c>
       <c r="E213" t="n">
-        <v>6.546</v>
+        <v>6.546492659053833</v>
       </c>
       <c r="F213" t="n">
-        <v>0.999</v>
+        <v>0.9985070913162478</v>
       </c>
       <c r="G213" s="2" t="n">
         <v>45657.80763888889</v>
@@ -7473,10 +7473,10 @@
         <v>3135</v>
       </c>
       <c r="E214" t="n">
-        <v>6.817</v>
+        <v>6.816993464052287</v>
       </c>
       <c r="F214" t="n">
-        <v>0.998</v>
+        <v>0.998086124401914</v>
       </c>
       <c r="G214" s="2" t="n">
         <v>45659.75486111111</v>
@@ -7498,10 +7498,10 @@
         <v>5371</v>
       </c>
       <c r="E215" t="n">
-        <v>6.268</v>
+        <v>6.267523364485982</v>
       </c>
       <c r="F215" t="n">
-        <v>0.999</v>
+        <v>0.9988828895922548</v>
       </c>
       <c r="G215" s="2" t="n">
         <v>45294.76666666667</v>
@@ -7523,10 +7523,10 @@
         <v>7887</v>
       </c>
       <c r="E216" t="n">
-        <v>6.651</v>
+        <v>6.650632911392405</v>
       </c>
       <c r="F216" t="n">
-        <v>0.999</v>
+        <v>0.99923925446938</v>
       </c>
       <c r="G216" s="2" t="n">
         <v>45676.70347222222</v>
@@ -7548,10 +7548,10 @@
         <v>5225</v>
       </c>
       <c r="E217" t="n">
-        <v>6.371</v>
+        <v>6.370689655172414</v>
       </c>
       <c r="F217" t="n">
-        <v>0.99</v>
+        <v>0.9900478468899522</v>
       </c>
       <c r="G217" s="2" t="n">
         <v>45678.74583333333</v>
@@ -7573,10 +7573,10 @@
         <v>14403</v>
       </c>
       <c r="E218" t="n">
-        <v>6.209</v>
+        <v>6.208796090626389</v>
       </c>
       <c r="F218" t="n">
-        <v>0.97</v>
+        <v>0.9703533985975143</v>
       </c>
       <c r="G218" s="2" t="n">
         <v>45689.79930555556</v>
@@ -7598,10 +7598,10 @@
         <v>4633</v>
       </c>
       <c r="E219" t="n">
-        <v>6.471</v>
+        <v>6.471328671328672</v>
       </c>
       <c r="F219" t="n">
-        <v>0.999</v>
+        <v>0.9987049428016403</v>
       </c>
       <c r="G219" s="2" t="n">
         <v>45692.77430555555</v>
@@ -7623,10 +7623,10 @@
         <v>8047</v>
       </c>
       <c r="E220" t="n">
-        <v>6.382</v>
+        <v>6.381746031746032</v>
       </c>
       <c r="F220" t="n">
-        <v>0.999</v>
+        <v>0.9992543805144776</v>
       </c>
       <c r="G220" s="2" t="n">
         <v>45699.72847222222</v>
@@ -7648,10 +7648,10 @@
         <v>5978</v>
       </c>
       <c r="E221" t="n">
-        <v>6.271</v>
+        <v>6.271186440677966</v>
       </c>
       <c r="F221" t="n">
-        <v>0.99</v>
+        <v>0.9902977584476412</v>
       </c>
       <c r="G221" s="2" t="n">
         <v>45706.75208333333</v>
@@ -7673,10 +7673,10 @@
         <v>11982</v>
       </c>
       <c r="E222" t="n">
-        <v>6.301</v>
+        <v>6.300703082747431</v>
       </c>
       <c r="F222" t="n">
-        <v>0.972</v>
+        <v>0.972291770989818</v>
       </c>
       <c r="G222" s="2" t="n">
         <v>45707.70347222222</v>
@@ -7698,10 +7698,10 @@
         <v>8694</v>
       </c>
       <c r="E223" t="n">
-        <v>6.228</v>
+        <v>6.227737226277372</v>
       </c>
       <c r="F223" t="n">
-        <v>0.981</v>
+        <v>0.9813664596273292</v>
       </c>
       <c r="G223" s="2" t="n">
         <v>45720.81319444445</v>
@@ -7723,10 +7723,10 @@
         <v>5913</v>
       </c>
       <c r="E224" t="n">
-        <v>6.359</v>
+        <v>6.358836206896552</v>
       </c>
       <c r="F224" t="n">
-        <v>0.998</v>
+        <v>0.9979705733130392</v>
       </c>
       <c r="G224" s="2" t="n">
         <v>45721.47986111111</v>
@@ -7748,10 +7748,10 @@
         <v>1326</v>
       </c>
       <c r="E225" t="n">
-        <v>7.663</v>
+        <v>7.662576687116564</v>
       </c>
       <c r="F225" t="n">
-        <v>0.9419999999999999</v>
+        <v>0.9419306184012066</v>
       </c>
       <c r="G225" s="2" t="n">
         <v>45553.76388888889</v>
@@ -7773,10 +7773,10 @@
         <v>7078</v>
       </c>
       <c r="E226" t="n">
-        <v>6.508</v>
+        <v>6.507518796992481</v>
       </c>
       <c r="F226" t="n">
-        <v>0.978</v>
+        <v>0.978242441367618</v>
       </c>
       <c r="G226" s="2" t="n">
         <v>45728.80694444444</v>
@@ -7798,10 +7798,10 @@
         <v>3599</v>
       </c>
       <c r="E227" t="n">
-        <v>6.26</v>
+        <v>6.26007326007326</v>
       </c>
       <c r="F227" t="n">
-        <v>0.95</v>
+        <v>0.9497082522923034</v>
       </c>
       <c r="G227" s="2" t="n">
         <v>45733.52847222222</v>
@@ -7823,10 +7823,10 @@
         <v>11640</v>
       </c>
       <c r="E228" t="n">
-        <v>6.743</v>
+        <v>6.743394010569583</v>
       </c>
       <c r="F228" t="n">
-        <v>0.987</v>
+        <v>0.9865979381443299</v>
       </c>
       <c r="G228" s="2" t="n">
         <v>45743.76180555556</v>
@@ -7848,10 +7848,10 @@
         <v>17675</v>
       </c>
       <c r="E229" t="n">
-        <v>6.069</v>
+        <v>6.069406077348066</v>
       </c>
       <c r="F229" t="n">
-        <v>0.994</v>
+        <v>0.9944554455445545</v>
       </c>
       <c r="G229" s="2" t="n">
         <v>45750.67916666667</v>
@@ -7873,10 +7873,10 @@
         <v>4043</v>
       </c>
       <c r="E230" t="n">
-        <v>5.916</v>
+        <v>5.916030534351145</v>
       </c>
       <c r="F230" t="n">
-        <v>0.958</v>
+        <v>0.9584466979965371</v>
       </c>
       <c r="G230" s="2" t="n">
         <v>45753.84375</v>
@@ -7895,16 +7895,16 @@
         <v>1058</v>
       </c>
       <c r="D231" t="n">
-        <v>6676</v>
+        <v>6675</v>
       </c>
       <c r="E231" t="n">
-        <v>6.198</v>
+        <v>6.196597353497165</v>
       </c>
       <c r="F231" t="n">
-        <v>0.982</v>
+        <v>0.9821722846441948</v>
       </c>
       <c r="G231" s="2" t="n">
-        <v>45878.675</v>
+        <v>45756.675</v>
       </c>
     </row>
     <row r="232">
@@ -7923,10 +7923,10 @@
         <v>14320</v>
       </c>
       <c r="E232" t="n">
-        <v>6.211</v>
+        <v>6.210595446584938</v>
       </c>
       <c r="F232" t="n">
-        <v>0.991</v>
+        <v>0.990572625698324</v>
       </c>
       <c r="G232" s="2" t="n">
         <v>45760.83819444444</v>
@@ -7948,10 +7948,10 @@
         <v>7039</v>
       </c>
       <c r="E233" t="n">
-        <v>6.435</v>
+        <v>6.434981684981685</v>
       </c>
       <c r="F233" t="n">
-        <v>0.998</v>
+        <v>0.9982952123881234</v>
       </c>
       <c r="G233" s="2" t="n">
         <v>45762.74791666667</v>
@@ -7973,10 +7973,10 @@
         <v>12437</v>
       </c>
       <c r="E234" t="n">
-        <v>6.17</v>
+        <v>6.169944528492184</v>
       </c>
       <c r="F234" t="n">
-        <v>0.984</v>
+        <v>0.9837581410307952</v>
       </c>
       <c r="G234" s="2" t="n">
         <v>45764.75694444445</v>
@@ -7998,10 +7998,10 @@
         <v>7857</v>
       </c>
       <c r="E235" t="n">
-        <v>6.193</v>
+        <v>6.192771084337349</v>
       </c>
       <c r="F235" t="n">
-        <v>0.981</v>
+        <v>0.9812905689194348</v>
       </c>
       <c r="G235" s="2" t="n">
         <v>45765.63125</v>
@@ -8020,16 +8020,116 @@
         <v>1107</v>
       </c>
       <c r="D236" t="n">
-        <v>7196</v>
+        <v>7197</v>
       </c>
       <c r="E236" t="n">
-        <v>6.467</v>
+        <v>6.467931345980126</v>
       </c>
       <c r="F236" t="n">
-        <v>0.995</v>
+        <v>0.9948589690148671</v>
       </c>
       <c r="G236" s="2" t="n">
         <v>45772.83472222222</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>1235</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Discussion Notes</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>3127</v>
+      </c>
+      <c r="D237" t="n">
+        <v>20007</v>
+      </c>
+      <c r="E237" t="n">
+        <v>6.306683722417652</v>
+      </c>
+      <c r="F237" t="n">
+        <v>0.9857050032488628</v>
+      </c>
+      <c r="G237" s="2" t="n">
+        <v>45617.75902777778</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>1236</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Discussion Notes</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>2407</v>
+      </c>
+      <c r="D238" t="n">
+        <v>14882</v>
+      </c>
+      <c r="E238" t="n">
+        <v>6.177814707104279</v>
+      </c>
+      <c r="F238" t="n">
+        <v>0.9991936567665636</v>
+      </c>
+      <c r="G238" s="2" t="n">
+        <v>45667.82083333333</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>1237</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Discussion Notes</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>881</v>
+      </c>
+      <c r="D239" t="n">
+        <v>5811</v>
+      </c>
+      <c r="E239" t="n">
+        <v>6.540295119182747</v>
+      </c>
+      <c r="F239" t="n">
+        <v>0.9915677163999312</v>
+      </c>
+      <c r="G239" s="2" t="n">
+        <v>45786.69027777778</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>1238</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Discussion Notes</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>1529</v>
+      </c>
+      <c r="D240" t="n">
+        <v>9601</v>
+      </c>
+      <c r="E240" t="n">
+        <v>6.221059516023545</v>
+      </c>
+      <c r="F240" t="n">
+        <v>0.9907301322778878</v>
+      </c>
+      <c r="G240" s="2" t="n">
+        <v>45794.79166666666</v>
       </c>
     </row>
   </sheetData>
@@ -8043,7 +8143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1161"/>
+  <dimension ref="A1:F1170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31283,6 +31383,186 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1162">
+      <c r="A1162" t="n">
+        <v>3408</v>
+      </c>
+      <c r="B1162" t="n">
+        <v>380</v>
+      </c>
+      <c r="C1162" s="2" t="n">
+        <v>45801.56623842593</v>
+      </c>
+      <c r="D1162" t="b">
+        <v>0</v>
+      </c>
+      <c r="E1162" t="n">
+        <v>15441</v>
+      </c>
+      <c r="F1162" t="n">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="n">
+        <v>3407</v>
+      </c>
+      <c r="B1163" t="n">
+        <v>380</v>
+      </c>
+      <c r="C1163" s="2" t="n">
+        <v>45801.55300925926</v>
+      </c>
+      <c r="D1163" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1163" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F1163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="n">
+        <v>3406</v>
+      </c>
+      <c r="B1164" t="n">
+        <v>380</v>
+      </c>
+      <c r="C1164" s="2" t="n">
+        <v>45801.54494212963</v>
+      </c>
+      <c r="D1164" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1164" t="n">
+        <v>14896</v>
+      </c>
+      <c r="F1164" t="n">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="n">
+        <v>3405</v>
+      </c>
+      <c r="B1165" t="n">
+        <v>380</v>
+      </c>
+      <c r="C1165" s="2" t="n">
+        <v>45801.53200231482</v>
+      </c>
+      <c r="D1165" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1165" t="n">
+        <v>20021</v>
+      </c>
+      <c r="F1165" t="n">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="n">
+        <v>3404</v>
+      </c>
+      <c r="B1166" t="n">
+        <v>555</v>
+      </c>
+      <c r="C1166" s="2" t="n">
+        <v>45801.53</v>
+      </c>
+      <c r="D1166" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1166" t="n">
+        <v>-73</v>
+      </c>
+      <c r="F1166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="n">
+        <v>3403</v>
+      </c>
+      <c r="B1167" t="n">
+        <v>326</v>
+      </c>
+      <c r="C1167" s="2" t="n">
+        <v>45801.52984953704</v>
+      </c>
+      <c r="D1167" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1167" t="n">
+        <v>-32</v>
+      </c>
+      <c r="F1167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="n">
+        <v>3401</v>
+      </c>
+      <c r="B1168" t="n">
+        <v>273</v>
+      </c>
+      <c r="C1168" s="2" t="n">
+        <v>45799.87296296296</v>
+      </c>
+      <c r="D1168" t="b">
+        <v>0</v>
+      </c>
+      <c r="E1168" t="n">
+        <v>1264</v>
+      </c>
+      <c r="F1168" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="n">
+        <v>3400</v>
+      </c>
+      <c r="B1169" t="n">
+        <v>208</v>
+      </c>
+      <c r="C1169" s="2" t="n">
+        <v>45798.94920138889</v>
+      </c>
+      <c r="D1169" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1169" t="n">
+        <v>-37</v>
+      </c>
+      <c r="F1169" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="n">
+        <v>3399</v>
+      </c>
+      <c r="B1170" t="n">
+        <v>269</v>
+      </c>
+      <c r="C1170" s="2" t="n">
+        <v>45798.8486574074</v>
+      </c>
+      <c r="D1170" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1170" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1170" t="n">
+        <v>-6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>